<commit_message>
Updated TRA to include hearing loss
</commit_message>
<xml_diff>
--- a/TRA EP.xlsx
+++ b/TRA EP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\Natuurkunde WO\Experimental-Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lotte\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02C455E-7C11-4181-AF51-C39EA45AE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AE620A-FC1C-4140-BAAC-80F064382EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TRA form (empty)" sheetId="3" r:id="rId1"/>
@@ -2385,7 +2385,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="99">
   <si>
     <t>Severity (S) </t>
   </si>
@@ -2674,6 +2674,21 @@
   </si>
   <si>
     <t>laser should always be aiming at a wall. Laser should be below eye level. Laser should be turned off when not in use. Laser warning sign and warning light should be on and present when laser in use</t>
+  </si>
+  <si>
+    <t>Working with sound &gt;85 dB</t>
+  </si>
+  <si>
+    <t>Hearing loss</t>
+  </si>
+  <si>
+    <t>Wear ear protection above 85 dB</t>
+  </si>
+  <si>
+    <t>Monitor sound level, avoid playing sound above 85 dB if not necessary, do not play sound above 100 dB</t>
+  </si>
+  <si>
+    <t>Immediately see a doctor</t>
   </si>
 </sst>
 </file>
@@ -3700,9 +3715,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
     <cellStyle name="Standaard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Standaard 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="60">
     <dxf>
@@ -4721,12 +4736,12 @@
   </sheetPr>
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" style="11" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" style="11" customWidth="1"/>
@@ -5832,30 +5847,54 @@
       </c>
       <c r="P9" s="39"/>
     </row>
-    <row r="10" spans="1:16" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="41">
         <v>4</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
+      <c r="B10" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="69">
+        <v>1</v>
+      </c>
+      <c r="E10" s="69">
+        <v>6</v>
+      </c>
+      <c r="F10" s="69">
+        <v>6</v>
+      </c>
       <c r="G10" s="56">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
+        <v>36</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" s="69">
+        <v>1</v>
+      </c>
+      <c r="K10" s="69">
+        <v>6</v>
+      </c>
+      <c r="L10" s="69">
+        <v>0.5</v>
+      </c>
       <c r="M10" s="56">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N10" s="17"/>
-      <c r="O10" s="45"/>
+        <v>3</v>
+      </c>
+      <c r="N10" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="O10" s="45" t="s">
+        <v>87</v>
+      </c>
       <c r="P10" s="39"/>
     </row>
     <row r="11" spans="1:16" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -6117,11 +6156,11 @@
   </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A5" zoomScale="107" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="20.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="38" style="1" customWidth="1"/>
@@ -7208,7 +7247,7 @@
       <selection pane="bottomLeft" activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" style="11" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" style="11" customWidth="1"/>
@@ -8599,7 +8638,7 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" style="11" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" style="11" customWidth="1"/>

</xml_diff>